<commit_message>
Panel class working, rough workings of downwash class
</commit_message>
<xml_diff>
--- a/resources/VLM_Coords.xlsx
+++ b/resources/VLM_Coords.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="174" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="349" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Example Wing" sheetId="1" state="visible" r:id="rId2"/>
@@ -89,6 +89,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -178,10 +179,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G31" activeCellId="0" sqref="E31:G31"/>
+      <selection pane="topLeft" activeCell="C38" activeCellId="0" sqref="C37:C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -532,13 +533,13 @@
       <c r="E21" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="F21" s="0" t="n">
-        <f aca="false">F11</f>
-        <v>0</v>
-      </c>
-      <c r="G21" s="0" t="n">
-        <f aca="false">G11-0.2*$B$3</f>
-        <v>-1</v>
+      <c r="F21" s="2" t="n">
+        <f aca="false">E21*$F$1</f>
+        <v>2.5</v>
+      </c>
+      <c r="G21" s="2" t="n">
+        <f aca="false">$G$11-F21*TAN(RADIANS($B$1))</f>
+        <v>-2.5</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -546,12 +547,12 @@
         <v>11</v>
       </c>
       <c r="F22" s="0" t="n">
-        <f aca="false">F12</f>
-        <v>0.25</v>
+        <f aca="false">F11</f>
+        <v>0</v>
       </c>
       <c r="G22" s="0" t="n">
-        <f aca="false">G12-0.2*$B$3</f>
-        <v>-1.25</v>
+        <f aca="false">G11-0.2*$B$3</f>
+        <v>-1</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -559,12 +560,12 @@
         <v>12</v>
       </c>
       <c r="F23" s="0" t="n">
-        <f aca="false">F13</f>
-        <v>0.5</v>
+        <f aca="false">F12</f>
+        <v>0.25</v>
       </c>
       <c r="G23" s="0" t="n">
-        <f aca="false">G13-0.2*$B$3</f>
-        <v>-1.5</v>
+        <f aca="false">G12-0.2*$B$3</f>
+        <v>-1.25</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -572,12 +573,12 @@
         <v>13</v>
       </c>
       <c r="F24" s="0" t="n">
-        <f aca="false">F14</f>
-        <v>0.75</v>
+        <f aca="false">F13</f>
+        <v>0.5</v>
       </c>
       <c r="G24" s="0" t="n">
-        <f aca="false">G14-0.2*$B$3</f>
-        <v>-1.75</v>
+        <f aca="false">G13-0.2*$B$3</f>
+        <v>-1.5</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -585,12 +586,12 @@
         <v>14</v>
       </c>
       <c r="F25" s="0" t="n">
-        <f aca="false">F15</f>
-        <v>1</v>
+        <f aca="false">F14</f>
+        <v>0.75</v>
       </c>
       <c r="G25" s="0" t="n">
-        <f aca="false">G15-0.2*$B$3</f>
-        <v>-2</v>
+        <f aca="false">G14-0.2*$B$3</f>
+        <v>-1.75</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -598,12 +599,12 @@
         <v>15</v>
       </c>
       <c r="F26" s="0" t="n">
-        <f aca="false">F16</f>
-        <v>1.25</v>
+        <f aca="false">F15</f>
+        <v>1</v>
       </c>
       <c r="G26" s="0" t="n">
-        <f aca="false">G16-0.2*$B$3</f>
-        <v>-2.25</v>
+        <f aca="false">G15-0.2*$B$3</f>
+        <v>-2</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -611,12 +612,12 @@
         <v>16</v>
       </c>
       <c r="F27" s="0" t="n">
-        <f aca="false">F17</f>
-        <v>1.5</v>
+        <f aca="false">F16</f>
+        <v>1.25</v>
       </c>
       <c r="G27" s="0" t="n">
-        <f aca="false">G17-0.2*$B$3</f>
-        <v>-2.5</v>
+        <f aca="false">G16-0.2*$B$3</f>
+        <v>-2.25</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -624,12 +625,12 @@
         <v>17</v>
       </c>
       <c r="F28" s="0" t="n">
-        <f aca="false">F18</f>
-        <v>1.75</v>
+        <f aca="false">F17</f>
+        <v>1.5</v>
       </c>
       <c r="G28" s="0" t="n">
-        <f aca="false">G18-0.2*$B$3</f>
-        <v>-2.75</v>
+        <f aca="false">G17-0.2*$B$3</f>
+        <v>-2.5</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -637,12 +638,12 @@
         <v>18</v>
       </c>
       <c r="F29" s="0" t="n">
-        <f aca="false">F19</f>
-        <v>2</v>
+        <f aca="false">F18</f>
+        <v>1.75</v>
       </c>
       <c r="G29" s="0" t="n">
-        <f aca="false">G19-0.2*$B$3</f>
-        <v>-3</v>
+        <f aca="false">G18-0.2*$B$3</f>
+        <v>-2.75</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -650,12 +651,12 @@
         <v>19</v>
       </c>
       <c r="F30" s="0" t="n">
-        <f aca="false">F20</f>
-        <v>2.25</v>
+        <f aca="false">F19</f>
+        <v>2</v>
       </c>
       <c r="G30" s="0" t="n">
-        <f aca="false">G20-0.2*$B$3</f>
-        <v>-3.25</v>
+        <f aca="false">G19-0.2*$B$3</f>
+        <v>-3</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -663,9 +664,35 @@
         <v>20</v>
       </c>
       <c r="F31" s="0" t="n">
-        <v>0</v>
+        <f aca="false">F20</f>
+        <v>2.25</v>
       </c>
       <c r="G31" s="0" t="n">
+        <f aca="false">G20-0.2*$B$3</f>
+        <v>-3.25</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E32" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="F32" s="0" t="n">
+        <f aca="false">F21</f>
+        <v>2.5</v>
+      </c>
+      <c r="G32" s="0" t="n">
+        <f aca="false">G21-0.2*$B$3</f>
+        <v>-3.5</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E33" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="F33" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G33" s="0" t="n">
         <v>-0.01</v>
       </c>
     </row>

</xml_diff>